<commit_message>
Added some exception handling
</commit_message>
<xml_diff>
--- a/Data/ProviderList.xlsx
+++ b/Data/ProviderList.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GabeJames\Documents\UiPath\EmailIntakeProcessing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F89CDB6-8FDA-4425-93E7-7AA3DD1C6091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8895B8FC-A279-4E81-9571-1D631A39A42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProviderToServicesMap" sheetId="4" r:id="rId1"/>
     <sheet name="Provider_Incurancecode" sheetId="1" r:id="rId2"/>
     <sheet name="InsuranceCarrierMapKey" sheetId="5" r:id="rId3"/>
     <sheet name="AppointmentTypeMap" sheetId="6" r:id="rId4"/>
+    <sheet name="EmailMap" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="373">
   <si>
     <t>NPI</t>
   </si>
@@ -1040,17 +1041,203 @@
   </si>
   <si>
     <t>Gift</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>[Brennan Behavior Group] Insurance Cards Needed</t>
+  </si>
+  <si>
+    <t>[Brennan Behavior Group] Credit Card Needed</t>
+  </si>
+  <si>
+    <t>Hi there-
+I'm processing your paperwork and for some reason, the credit card information is failing to verify. You are not being charged for any services at this time. It is our office policy to have a card on file prior to scheduling any appointments.You can give us a call at 504-833-6730 anytime between 9 a.m. and 4:30 p.m. to verify the card information or you can submit a credit card form through the link below. 
+Credit Card From: https://app.goformz.com/s/UNaeaF0C3T4CMrLMQ</t>
+  </si>
+  <si>
+    <t>Credit Card Error</t>
+  </si>
+  <si>
+    <t>Credit Card Missing</t>
+  </si>
+  <si>
+    <t>Hi there-
+I'm processing your paperwork and see that you did not fill out the credit card form.You are not being charged for any services at this time. It is our office policy to have a card on file prior to scheduling any appointments. You can submit a credit card form through the link below.
+Credit Card From: https://app.goformz.com/s/UNaeaF0C3T4CMrLMQ
+If you'd prefer to give us the card information over the phone, you can call us at 504-833-6730 anytime between 9 a.m. and 4:30 p.m. Please let me know if you have any questions.
+Best,</t>
+  </si>
+  <si>
+    <t>Custody Agreement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Brennan Behavior Group] Custody Agreement </t>
+  </si>
+  <si>
+    <t>Hi there, 
+I am processing your paperwork right now and see that you confirmed a custody agreement is in place for the patient. We would need a copy of the legal document stating the custody judgment before we can proceed with scheduling. 
+Best,</t>
+  </si>
+  <si>
+    <t>[Brennan Behavior Group] ABA New Patient Paperwork</t>
+  </si>
+  <si>
+    <t>Hi,
+Thank you for your interest in Brennan Behavior Group!
+I am reaching out because I see you have submitted your information through our website for ABA therapy. In order to complete your profile and get your child on the waitlist, I will need all of the following documents completed and turned in. Your child will not be in line for ABA services until all paperwork is received. 
+First, I will need this questionnaire completed. It will help our providers determine your child’s specific needs a little better.
+Parent Questionnaire: https://forms.gle/te9G6SZHfGkDXLgP9
+Next, I will need these documents:
+A copy of your child’s diagnosis report. I will need the full packet complete with your child’s name and the doctor’s signature. I prefer this in PDF format
+ A picture of the front and back of your child’s insurance card.
+A copy of our ABA intake paperwork completed and returned. This will be linked below for you to fill out. Once you fill it out and finish, it will automatically submit it to us.
+Link to the ABA paperwork:
+https://app.goformz.com/s/1MdG5YD51RRRvTsP6MQ
+Again, please do not hesitate to let me know if you have any questions!</t>
+  </si>
+  <si>
+    <t>[Brennan Behavior Group] Self Pay Consent</t>
+  </si>
+  <si>
+    <t>I'm processing your paperwork right now and see that you left the insurance section blank. If you'd like to proceed with self-pay please let me know! Below is the 2025 self-pay pricing list for our testing services. Billing for evaluations is reviewed with you and collected at the end of the process which is post testing.
+For self-pay patients a $300 Clinical Interview
+balance will be charged to the credit card on file on the day of the Clinical Interview appointment. The remaining evaluation balance will be charged to the card on file at the time of the feedback
+appointment. Educational testing will never be covered by insurance, which I’ve indicated in parentheses below.
+ADHD Testing — $2,460.00
+ASD Testing — $2,460.00-2,890.00
+Clergy/Seminarian Testing — $1950.00
+Psychoeducational/Full Evaluation — $3,305.00 ($1,750.00 is not covered by insurance)
+Gifted/IQ — $696.00 (not covered by insurance)
+Clinical Interview/Consultation (included in the above prices, but just the appointment alone) — $300.00 Billed after Clinical Interview.
+Please let me know if you have any questions and how you would like to proceed.
+Best,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couples Therapy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Brennan Behavior Group] Couples Therapy </t>
+  </si>
+  <si>
+    <t>Hi there- 
+I see that you are interested in doing couples therapy. Our couples therapy is done by Ms. Lydia Jaunet, is an hour-long session, and is not covered by insurance. The cost of couples therapy is $250 a session. If you are interested in proceeding please have each partner complete the paperwork below and return it to this email address. Please don't hesitate to contact me if you have any questions or concerns!
+The link to fill out paperwork is below:
+https://app.goformz.com/s/Euj0YqkSiAugQqv6Ijr</t>
+  </si>
+  <si>
+    <t>Therapy Adult</t>
+  </si>
+  <si>
+    <t>[Brennan Behavior Group] Therapy Providers</t>
+  </si>
+  <si>
+    <t>Hi there-
+I am processing your paperwork and Ms. Amy Alvarez is our only adult therapist. She does accept insurance, but she has a waitlist of about 3-4 months. Amy has a special interest in prenatal and postpartum mental health, infant/toddler parenting support, infertility, and adoption. She also enjoys working with clients coping with divorce/custody, step-families, and career issues. Amy is LGBTQ allied and committed to social justice.
+Please let me know if you have any questions!
+Best,</t>
+  </si>
+  <si>
+    <t>Therapy Teens</t>
+  </si>
+  <si>
+    <t>Hi there-
+I am processing your paperwork and I wanted to reach out and give you some options as far as therapy providers. Unfortunately, we do not allow patients to be on multiple waitlists for providers at a time so once you review please let us know your preferred choice. 
+The first would be Ms. Lydia Jaunet. She does accept insurance, however, she is on a waitlist of about 4-6 months.  Lydia has experience in treating individuals, couples, and families who are struggling with disruptive behavior, conduct issues, ADD/ADHD, anxiety, depression, self-harming behaviors, and personality disorders.  Lydia strives to provide exceptional services through individual interventions based on her client’s needs, solution-focused treatment,  and cognitive-behavioral treatment models. 
+The other option would be Ms. Maya Gisclair. She does not accept insurance. Her self-pay rate is $138 for the very first session and any 60 minute sessions and $70 for each 30-minute session following that. She is on a waitlist of about 3-4 months. Maya addresses a wide range of psychological and behavioral issues through the use of functional communication training, solution-focused and client-centered treatment plans, as well as utilizing some Cognitive Behavioral Therapy (CBT) models. Her professional interests include ASD, disruptive behavior, conduct issues, ADD/ADHD, anxiety, depression, and self-injurious behaviors.
+The other option would be Ms. Amie Johnson. She is on a waitlist of 2-3 months, but she does not accept insurance. Her rates are $138 for the initial appointment, $138 for 60-minute sessions and $70 for 30-minute sessions. Amie’s interest is in providing therapeutic services to children, adolescents, and young-adults who are facing symptoms of depression, anxiety, ADD/ADHD, and ASD behaviors.                                                                                                                                                                              Please let me know if you have any other questions!
+Best,</t>
+  </si>
+  <si>
+    <t>Therapy Children</t>
+  </si>
+  <si>
+    <t>Hi there, 
+I am processing your paperwork and I wanted to reach out and give you some options as far as therapy providers. Unfortunately, we do not allow patients to be on multiple waitlists for providers at a time so once you review please let us know your preferred choice.  
+The first would be Ms. Lydia Jaunet. She does accept insurance, however, she is on a waitlist of about 4-6 months.  Lydia has experience in treating individuals, couples, and families who are struggling with disruptive behavior, conduct issues, ADD/ADHD, anxiety, depression, self-harming behaviors, and personality disorders.  Lydia strives to provide exceptional services through individual interventions based on her client’s needs, solution-focused treatment, and cognitive-behavioral treatment models. 
+The other option would be Ms. Maya Gisclair. She does not accept insurance. Her self-pay rate is $138 for the very first session and $70 for each 30-minute session following that.  She is on a waitlist of about 3-4 months. Maya addresses a wide range of psychological and behavioral issues through the use of functional communication training, solution-focused and client-centered treatment plans, as well as utilizing some Cognitive Behavioral Therapy (CBT) models. Her professional interests include ASD, disruptive behavior, conduct issues, ADD/ADHD, anxiety, depression, and self-injurious behaviors.                                                                                                                                                                                                                                            Please let me know if you have any other questions!
+Best,</t>
+  </si>
+  <si>
+    <t>Self Pay Blank</t>
+  </si>
+  <si>
+    <t>Self Pay Medicaid</t>
+  </si>
+  <si>
+    <t>I'm processing your paperwork right now and see that the insurance that you have provided us is an insurance we do not accept. If you'd like to proceed with self-pay please let me know! Below is the 2025 self-pay pricing list for our testing services. Billing for evaluations is reviewed with you and collected at the end of the process which is post testing.
+For self-pay patients a $300 Clinical Interview
+balance will be charged to the credit card on file on the day of the Clinical Interview appointment. The remaining evaluation balance will be charged to the card on file at the time of the feedback
+appointment. Educational testing will never be covered by insurance, which I’ve indicated in parentheses below.
+ADHD Testing — $2,460.00
+ASD Testing — $2,460.00-2,890.00
+Clergy/Seminarian Testing — $1950.00
+Psychoeducational/Full Evaluation — $3,305.00 ($1,750.00 is not covered by insurance)
+Gifted/IQ — $696.00 (not covered by insurance)
+Clinical Interview/Consultation (included in the above prices, but just the appointment alone) — $300.00 Billed after Clinical Interview.
+Please let me know if you have any questions and how you would like to proceed.
+Best,</t>
+  </si>
+  <si>
+    <t>[Brennan Behavior Group] Clerical Evaluation</t>
+  </si>
+  <si>
+    <t>Hi there,
+We see that you are interested in being evaluated by Dr. Gallagher. The paperwork attached to this email is our next step  in getting an appointment set up. It is preliminary information required for the evaluation. Once we receive the attached paperwork back, we will reach out with some appointment availability. Please let me know if you have any questions or concerns along the way!
+The link to the paperwork is below:
+https://app.goformz.com/s/9kY1p2UAnd4drPhNOHmw
+Best,</t>
+  </si>
+  <si>
+    <t>Hi there- &lt;br/&gt;
+I'm processing your paperwork and it looks like we're just missing your insurance information. If you could send me a photo/copy of the front and back of your card that would be great!
+&lt;br/&gt;
+Best,</t>
+  </si>
+  <si>
+    <t>Therapy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1146,6 +1333,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1215,7 +1414,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1295,185 +1494,218 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2554,7 +2786,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -35171,7 +35403,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35347,10 +35579,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19B76EF-91B0-42FA-B349-2655AF5B2BBC}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35471,6 +35703,177 @@
         <v>318</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>372</v>
+      </c>
+      <c r="B15" t="s">
+        <v>318</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21507685-9379-4BA4-B5A0-8A2C4C5B5836}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.7265625" customWidth="1"/>
+    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="71" t="s">
+        <v>342</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>343</v>
+      </c>
+      <c r="C2" s="78" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="74" t="s">
+        <v>346</v>
+      </c>
+      <c r="B3" s="75" t="s">
+        <v>344</v>
+      </c>
+      <c r="C3" s="73" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="80" t="s">
+        <v>347</v>
+      </c>
+      <c r="B4" s="72" t="s">
+        <v>344</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="75" t="s">
+        <v>349</v>
+      </c>
+      <c r="B5" s="72" t="s">
+        <v>350</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="76" t="s">
+        <v>334</v>
+      </c>
+      <c r="B6" s="74" t="s">
+        <v>352</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="76" t="s">
+        <v>366</v>
+      </c>
+      <c r="B7" s="72" t="s">
+        <v>354</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="79" t="s">
+        <v>367</v>
+      </c>
+      <c r="B8" s="72" t="s">
+        <v>354</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="74" t="s">
+        <v>356</v>
+      </c>
+      <c r="B9" s="74" t="s">
+        <v>357</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="74" t="s">
+        <v>359</v>
+      </c>
+      <c r="B10" s="74" t="s">
+        <v>360</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="74" t="s">
+        <v>362</v>
+      </c>
+      <c r="B11" s="74" t="s">
+        <v>360</v>
+      </c>
+      <c r="C11" s="73" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="74" t="s">
+        <v>364</v>
+      </c>
+      <c r="B12" s="74" t="s">
+        <v>360</v>
+      </c>
+      <c r="C12" s="77" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="74" t="s">
+        <v>330</v>
+      </c>
+      <c r="B13" s="74" t="s">
+        <v>369</v>
+      </c>
+      <c r="C13" s="73" t="s">
+        <v>370</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed more exception handling and got running for 60%
</commit_message>
<xml_diff>
--- a/Data/ProviderList.xlsx
+++ b/Data/ProviderList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GabeJames\Documents\UiPath\EmailIntakeProcessing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8895B8FC-A279-4E81-9571-1D631A39A42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F92AD3-48F6-4646-9BD8-48BC7F0E1B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42444" yWindow="-2976" windowWidth="18720" windowHeight="11652" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProviderToServicesMap" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="373">
   <si>
     <t>NPI</t>
   </si>
@@ -1212,11 +1212,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1513,199 +1520,200 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2071,10 +2079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD75AEF6-164A-492E-8A25-0BD405F14B2D}">
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2262,7 +2270,7 @@
         <v>274</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -2288,28 +2296,20 @@
       <c r="K4" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="L4" s="52" t="s">
-        <v>277</v>
-      </c>
+      <c r="L4" s="52"/>
       <c r="M4" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="N4" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="O4" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q4" s="52" t="s">
-        <v>277</v>
-      </c>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="Q4" s="52"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="52" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -2329,31 +2329,35 @@
       <c r="I5" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="J5" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="K5" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="L5" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="M5" s="52" t="s">
-        <v>277</v>
-      </c>
+      <c r="M5" s="52"/>
       <c r="N5" s="52" t="s">
         <v>277</v>
       </c>
       <c r="O5" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="P5" s="52" t="s">
+      <c r="Q5" s="52" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="52" t="s">
-        <v>321</v>
+        <v>273</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
       <c r="C6">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
         <v>263</v>
@@ -2373,25 +2377,28 @@
       <c r="L6" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="M6" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="N6" s="52" t="s">
         <v>277</v>
       </c>
       <c r="O6" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="S6" s="52" t="s">
+      <c r="P6" s="52" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="52" t="s">
-        <v>276</v>
+        <v>321</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>263</v>
@@ -2411,19 +2418,25 @@
       <c r="L7" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="N7" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="O7" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="S7" s="52" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="52" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="D8" t="s">
         <v>263</v>
@@ -2440,28 +2453,22 @@
       <c r="I8" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="J8" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="K8" s="52" t="s">
-        <v>277</v>
-      </c>
       <c r="L8" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="M8" s="52" t="s">
+      <c r="O8" s="52" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="52" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B9">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>263</v>
@@ -2484,11 +2491,10 @@
       <c r="K9" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="L9" s="52"/>
+      <c r="L9" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="M9" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="O9" s="52" t="s">
         <v>277</v>
       </c>
     </row>
@@ -2497,10 +2503,10 @@
         <v>279</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="C10">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
         <v>263</v>
@@ -2523,7 +2529,8 @@
       <c r="K10" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="L10" s="52" t="s">
+      <c r="L10" s="52"/>
+      <c r="M10" s="52" t="s">
         <v>277</v>
       </c>
       <c r="O10" s="52" t="s">
@@ -2532,13 +2539,13 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="52" t="s">
-        <v>27</v>
+        <v>279</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>263</v>
@@ -2564,28 +2571,19 @@
       <c r="L11" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="M11" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="N11" s="52" t="s">
-        <v>277</v>
-      </c>
       <c r="O11" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="P11" s="52" t="s">
-        <v>277</v>
-      </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="52" t="s">
-        <v>280</v>
+        <v>27</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
         <v>263</v>
@@ -2602,28 +2600,40 @@
       <c r="I12" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="J12" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="K12" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="L12" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="M12" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="N12" s="52" t="s">
         <v>277</v>
       </c>
       <c r="O12" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="P12" s="52" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="52" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>25</v>
-      </c>
-      <c r="D13" s="52" t="s">
-        <v>283</v>
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>263</v>
       </c>
       <c r="F13" s="52" t="s">
         <v>277</v>
@@ -2631,35 +2641,31 @@
       <c r="G13" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="H13" s="52"/>
+      <c r="H13" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="I13" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="J13" s="52" t="s">
+      <c r="L13" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="T13" s="52" t="s">
+      <c r="N13" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="U13" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="V13" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="W13" s="52" t="s">
+      <c r="O13" s="52" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
         <v>18</v>
-      </c>
-      <c r="C14">
-        <v>100</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>283</v>
@@ -2670,25 +2676,26 @@
       <c r="G14" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="H14" s="52"/>
       <c r="I14" s="52" t="s">
         <v>277</v>
       </c>
       <c r="J14" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="K14" s="52" t="s">
+      <c r="T14" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="L14" s="52" t="s">
-        <v>277</v>
-      </c>
+      <c r="U14" s="52"/>
+      <c r="V14" s="52"/>
+      <c r="W14" s="52"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="52" t="s">
-        <v>325</v>
+        <v>281</v>
       </c>
       <c r="B15">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>100</v>
@@ -2702,25 +2709,33 @@
       <c r="G15" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="H15" s="52"/>
       <c r="I15" s="52" t="s">
         <v>277</v>
       </c>
       <c r="J15" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="T15" s="52" t="s">
+      <c r="T15" s="52"/>
+      <c r="U15" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="V15" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="W15" s="52" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="52" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C16">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="D16" s="52" t="s">
         <v>283</v>
@@ -2728,22 +2743,31 @@
       <c r="F16" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="G16" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="I16" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="T16" s="52" t="s">
+      <c r="J16" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="K16" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="L16" s="52" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="52" t="s">
-        <v>288</v>
+        <v>325</v>
       </c>
       <c r="B17">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C17">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="D17" s="52" t="s">
         <v>283</v>
@@ -2751,24 +2775,76 @@
       <c r="F17" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="G17" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="I17" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="J17" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="T17" s="52" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="T18" s="52"/>
+      <c r="A18" s="52" t="s">
+        <v>287</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>18</v>
+      </c>
+      <c r="D18" s="52" t="s">
+        <v>283</v>
+      </c>
+      <c r="F18" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="I18" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="T18" s="52" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="T19" s="52"/>
+      <c r="A19" s="52" t="s">
+        <v>288</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>23</v>
+      </c>
+      <c r="D19" s="52" t="s">
+        <v>283</v>
+      </c>
+      <c r="F19" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="I19" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="T19" s="52" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="T20" s="52"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="T21" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35720,15 +35796,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21507685-9379-4BA4-B5A0-8A2C4C5B5836}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.7265625" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -35775,8 +35851,8 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="75" t="s">
+    <row r="5" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="81" t="s">
         <v>349</v>
       </c>
       <c r="B5" s="72" t="s">

</xml_diff>

<commit_message>
Fixed some bugs and started fastgem intake
</commit_message>
<xml_diff>
--- a/Data/ProviderList.xlsx
+++ b/Data/ProviderList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GabeJames\Documents\UiPath\EmailIntakeProcessing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F92AD3-48F6-4646-9BD8-48BC7F0E1B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641FE114-9495-4284-8F20-CC9B9E996967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42444" yWindow="-2976" windowWidth="18720" windowHeight="11652" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProviderToServicesMap" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="374">
   <si>
     <t>NPI</t>
   </si>
@@ -1061,151 +1061,121 @@
     <t>[Brennan Behavior Group] Credit Card Needed</t>
   </si>
   <si>
+    <t>Credit Card Error</t>
+  </si>
+  <si>
+    <t>Credit Card Missing</t>
+  </si>
+  <si>
+    <t>Custody Agreement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Brennan Behavior Group] Custody Agreement </t>
+  </si>
+  <si>
+    <t>[Brennan Behavior Group] ABA New Patient Paperwork</t>
+  </si>
+  <si>
+    <t>[Brennan Behavior Group] Self Pay Consent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couples Therapy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Brennan Behavior Group] Couples Therapy </t>
+  </si>
+  <si>
+    <t>Therapy Adult</t>
+  </si>
+  <si>
+    <t>[Brennan Behavior Group] Therapy Providers</t>
+  </si>
+  <si>
+    <t>Therapy Teens</t>
+  </si>
+  <si>
+    <t>Therapy Children</t>
+  </si>
+  <si>
+    <t>Self Pay Blank</t>
+  </si>
+  <si>
+    <t>Self Pay Medicaid</t>
+  </si>
+  <si>
+    <t>[Brennan Behavior Group] Clerical Evaluation</t>
+  </si>
+  <si>
+    <t>Therapy</t>
+  </si>
+  <si>
+    <t>Hi there-&lt;br/&gt;&lt;br/&gt;I’m processing your paperwork and it looks like we’re just missing your insurance information. If you could send me a photo/copy of the front and back of your card that would be great!&lt;br/&gt;&lt;br/&gt;Best,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Hi there-&lt;br/&gt;&lt;br/&gt;I’m processing your paperwork and for some reason, the credit card information is failing to verify. You are not being charged for any services at this time. It is our office policy to have a card on file prior to scheduling any appointments. You can give us a call at 504‑833‑6730 anytime between 9 a.m. and 4:30 p.m. to verify the card information or you can submit a credit card form through the link below.&lt;br/&gt;&lt;br/&gt;&lt;mark&gt;Credit Card Form: https://app.goformz.com/s/UNaeaF0C3T4CMrLMQ&lt;/mark&gt;&lt;br/&gt;&lt;br/&gt;Best,</t>
+  </si>
+  <si>
+    <t>Hi,&lt;br/&gt;&lt;br/&gt;Thank you for your interest in Brennan Behavior Group!&lt;br/&gt;&lt;br/&gt;I am reaching out because I see you have submitted your information through our website for ABA therapy. In order to complete your profile and get your child on the waitlist, I will need all of the following documents completed and turned in. &lt;mark&gt;Your child will not be in line for ABA services until all paperwork is received.&lt;/mark&gt;&lt;br/&gt;&lt;br/&gt;First, I will need this questionnaire completed. It will help our providers determine your child’s specific needs a little better.&lt;br/&gt;&lt;mark&gt;Parent Questionnaire: https://forms.gle/te9G6SZHfGkDXLgP9&lt;/mark&gt;&lt;br/&gt;&lt;br/&gt;Next, I will need these documents:&lt;br/&gt;&lt;ul&gt;&lt;li&gt;A copy of your child’s diagnosis report. I will need the full packet complete with your child’s name and the doctor’s signature. I prefer this in PDF format&lt;/li&gt;&lt;li&gt;A picture of the front and back of your child’s insurance card.&lt;/li&gt;&lt;li&gt;A copy of our ABA intake paperwork completed and returned. This will be linked below for you to fill out. Once you fill it out and finish, it will automatically submit it to us.&lt;/li&gt;&lt;/ul&gt;&lt;br/&gt;Link to the ABA paperwork:&lt;br/&gt;&lt;mark&gt;https://app.goformz.com/s/1MdG5YD51RRRvTsP6MQ&lt;/mark&gt;&lt;br/&gt;&lt;br/&gt;Again, please do not hesitate to let me know if you have any questions!</t>
+  </si>
+  <si>
+    <t>Hi there, &lt;br/&gt;&lt;br/&gt;
+I am processing your paperwork right now and see that you confirmed a custody agreement is in place for the patient. We would need a copy of the legal document stating the custody judgment before we can proceed with scheduling. 
+&lt;br/&gt;&lt;br/&gt;
+Best,</t>
+  </si>
+  <si>
+    <t>Hi there-&lt;br/&gt;&lt;br/&gt;I’m processing your paperwork and for some reason, the credit card information is failing to verify. You are not being charged for any services at this time. It is our office policy to have a card on file prior to scheduling any appointments. You can give us a call at 504‑833‑6730 anytime between 9 a.m. and 4:30 p.m. to verify the card information or you can submit a credit card form through the link below.&lt;br/&gt;&lt;br/&gt;&lt;mark&gt;Credit Card Form: https://app.goformz.com/s/UNaeaF0C3T4CMrLMQ&lt;/mark&gt;&lt;br/&gt;&lt;br/&gt;Best,</t>
+  </si>
+  <si>
+    <t>Hi there-&lt;br/&gt;&lt;br/&gt;I’m processing your paperwork and see that you did not fill out the credit card form. &lt;strong&gt;You are not being charged for any services at this time.&lt;/strong&gt; It is our office policy to have a card on file prior to scheduling any appointments. You can submit a credit card form through the link below.&lt;br/&gt;&lt;br/&gt;&lt;mark&gt;Credit Card Form: https://app.goformz.com/s/UNaeaF0C3T4CMrLMQ&lt;/mark&gt;&lt;br/&gt;&lt;br/&gt;If you’d prefer to give us the card information over the phone, you can call us at 504‑833‑6730 anytime between 9 a.m. and 4:30 p.m. Please let me know if you have any questions.&lt;br/&gt;&lt;br/&gt;Best,</t>
+  </si>
+  <si>
+    <t>Hi there-&lt;br/&gt;&lt;br/&gt;I’m processing your paperwork right now and see that you left the insurance section blank. If you’d like to proceed with self‑pay please let me know! Below is the 2025 self‑pay pricing list for our testing services. &lt;strong&gt;Billing for evaluations is reviewed with you and collected at the end of the process which is post testing.&lt;/strong&gt;&lt;br/&gt;&lt;br/&gt;For self‑pay patients, a $300 Clinical Interview balance will be charged to the credit card on file on the day of the Clinical Interview appointment. The remaining evaluation balance will be charged to the card on file at the time of the feedback appointment. Educational testing will never be covered by insurance, which I’ve indicated in parentheses below.&lt;br/&gt;&lt;br/&gt;&lt;mark&gt;ADHD Testing — $2,460.00&lt;/mark&gt;&lt;br/&gt;&lt;mark&gt;ASD Testing — $2,460.00–2,890.00&lt;/mark&gt;&lt;br/&gt;&lt;mark&gt;Clergy/Seminarian Testing — $1,950.00&lt;/mark&gt;&lt;br/&gt;&lt;mark&gt;Psychoeducational/Full Evaluation — $3,305.00 ( $1,750.00 is not covered by insurance)&lt;/mark&gt;&lt;br/&gt;&lt;mark&gt;Gifted/IQ — $696.00 (not covered by insurance)&lt;/mark&gt;&lt;br/&gt;&lt;mark&gt;Clinical Interview/Consultation (included in the above prices, but just the appointment alone) — $300.00 Billed after Clinical Interview&lt;/mark&gt;&lt;br/&gt;&lt;br/&gt;Please let me know if you have any questions and how you would like to proceed.&lt;br/&gt;&lt;br/&gt;Best,</t>
+  </si>
+  <si>
+    <t>Hi there-&lt;br/&gt;&lt;br/&gt;I see that you are interested in doing couples therapy. Our couples therapy is done by Ms. Lydia Jaunet, is an hour‑long session, and is not covered by insurance. The cost of couples therapy is $250 a session. If you are interested in proceeding please have each partner complete the paperwork below and return it to this email address. Please don’t hesitate to contact me if you have any questions or concerns!&lt;br/&gt;&lt;br/&gt;The link to fill out paperwork is below:&lt;br/&gt;&lt;mark&gt;https://app.goformz.com/s/Euj0YqkSiAugQqv6Ijr&lt;/mark&gt;&lt;br/&gt;&lt;br/&gt;Best,</t>
+  </si>
+  <si>
+    <t>Hi there-&lt;br/&gt;&lt;br/&gt;
+I am processing your paperwork and Ms. Amy Alvarez is our only adult therapist. She does accept insurance, but she has a waitlist of about 3-4 months. Amy has a special interest in prenatal and postpartum mental health, infant/toddler parenting support, infertility, and adoption. She also enjoys working with clients coping with divorce/custody, step-families, and career issues. Amy is LGBTQ allied and committed to social justice.
+&lt;br/&gt;&lt;br/&gt;
+Please let me know if you have any questions!
+&lt;br/&gt;&lt;br/&gt;
+Best,</t>
+  </si>
+  <si>
+    <t>Hi there, 
+&lt;br/&gt;&lt;br/&gt;
+I am processing your paperwork and I wanted to reach out and give you some options as far as therapy providers. Unfortunately, we do not allow patients to be on multiple waitlists for providers at a time so once you review please let us know your preferred choice.  
+&lt;br/&gt;&lt;br/&gt;
+The first would be Ms. Lydia Jaunet. She does accept insurance, however, she is on a waitlist of about 4-6 months.  Lydia has experience in treating individuals, couples, and families who are struggling with disruptive behavior, conduct issues, ADD/ADHD, anxiety, depression, self-harming behaviors, and personality disorders.  Lydia strives to provide exceptional services through individual interventions based on her client’s needs, solution-focused treatment, and cognitive-behavioral treatment models. 
+&lt;br/&gt;&lt;br/&gt;
+The other option would be Ms. Maya Gisclair. She does not accept insurance. Her self-pay rate is $138 for the very first session and $70 for each 30-minute session following that.  She is on a waitlist of about 3-4 months. Maya addresses a wide range of psychological and behavioral issues through the use of functional communication training, solution-focused and client-centered treatment plans, as well as utilizing some Cognitive Behavioral Therapy (CBT) models. Her professional interests include ASD, disruptive behavior, conduct issues, ADD/ADHD, anxiety, depression, and self-injurious behaviors.            &lt;br/&gt;&lt;br/&gt;                                                                                                                                                                                                                                Please let me know if you have any other questions!
+&lt;br/&gt;&lt;br/&gt;
+Best,</t>
+  </si>
+  <si>
+    <t>Hi there,
+&lt;br/&gt;&lt;br/&gt;
+We see that you are interested in being evaluated by Dr. Gallagher. The paperwork attached to this email is our next step  in getting an appointment set up. It is preliminary information required for the evaluation. Once we receive the attached paperwork back, we will reach out with some appointment availability. Please let me know if you have any questions or concerns along the way!
+&lt;br/&gt;&lt;br/&gt;
+The link to the paperwork is below:&lt;br/&gt;
+https://app.goformz.com/s/9kY1p2UAnd4drPhNOHmw
+&lt;br/&gt;&lt;br/&gt;
+Best,</t>
+  </si>
+  <si>
     <t>Hi there-
-I'm processing your paperwork and for some reason, the credit card information is failing to verify. You are not being charged for any services at this time. It is our office policy to have a card on file prior to scheduling any appointments.You can give us a call at 504-833-6730 anytime between 9 a.m. and 4:30 p.m. to verify the card information or you can submit a credit card form through the link below. 
-Credit Card From: https://app.goformz.com/s/UNaeaF0C3T4CMrLMQ</t>
-  </si>
-  <si>
-    <t>Credit Card Error</t>
-  </si>
-  <si>
-    <t>Credit Card Missing</t>
-  </si>
-  <si>
-    <t>Hi there-
-I'm processing your paperwork and see that you did not fill out the credit card form.You are not being charged for any services at this time. It is our office policy to have a card on file prior to scheduling any appointments. You can submit a credit card form through the link below.
-Credit Card From: https://app.goformz.com/s/UNaeaF0C3T4CMrLMQ
-If you'd prefer to give us the card information over the phone, you can call us at 504-833-6730 anytime between 9 a.m. and 4:30 p.m. Please let me know if you have any questions.
+I am processing your paperwork and I wanted to reach out and give you some options as far as therapy providers. Unfortunately, we do not allow patients to be on multiple waitlists for providers at a time so once you review please let us know your preferred choice. &lt;br/&gt;&lt;br/&gt;
+The first would be Ms. Lydia Jaunet. She does accept insurance, however, she is on a waitlist of about 4-6 months.  Lydia has experience in treating individuals, couples, and families who are struggling with disruptive behavior, conduct issues, ADD/ADHD, anxiety, depression, self-harming behaviors, and personality disorders.  Lydia strives to provide exceptional services through individual interventions based on her client’s needs, solution-focused treatment,  and cognitive-behavioral treatment models. 
+&lt;br/&gt;&lt;br/&gt;
+The other option would be Ms. Maya Gisclair. She does not accept insurance. Her self-pay rate is $138 for the very first session and any 60 minute sessions and $70 for each 30-minute session following that. She is on a waitlist of about 3-4 months. Maya addresses a wide range of psychological and behavioral issues through the use of functional communication training, solution-focused and client-centered treatment plans, as well as utilizing some Cognitive Behavioral Therapy (CBT) models. Her professional interests include ASD, disruptive behavior, conduct issues, ADD/ADHD, anxiety, depression, and self-injurious behaviors.
+&lt;br/&gt;&lt;br/&gt;
+The other option would be Ms. Amie Johnson. She is on a waitlist of 2-3 months, but she does not accept insurance. Her rates are $138 for the initial appointment, $138 for 60-minute sessions and $70 for 30-minute sessions. Amie’s interest is in providing therapeutic services to children, adolescents, and young-adults who are facing symptoms of depression, anxiety, ADD/ADHD, and ASD behaviors.                    &lt;br/&gt;&lt;br/&gt;                                                                                                                                                          Please let me know if you have any other questions!
 Best,</t>
   </si>
   <si>
-    <t>Custody Agreement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Brennan Behavior Group] Custody Agreement </t>
-  </si>
-  <si>
-    <t>Hi there, 
-I am processing your paperwork right now and see that you confirmed a custody agreement is in place for the patient. We would need a copy of the legal document stating the custody judgment before we can proceed with scheduling. 
-Best,</t>
-  </si>
-  <si>
-    <t>[Brennan Behavior Group] ABA New Patient Paperwork</t>
-  </si>
-  <si>
-    <t>Hi,
-Thank you for your interest in Brennan Behavior Group!
-I am reaching out because I see you have submitted your information through our website for ABA therapy. In order to complete your profile and get your child on the waitlist, I will need all of the following documents completed and turned in. Your child will not be in line for ABA services until all paperwork is received. 
-First, I will need this questionnaire completed. It will help our providers determine your child’s specific needs a little better.
-Parent Questionnaire: https://forms.gle/te9G6SZHfGkDXLgP9
-Next, I will need these documents:
-A copy of your child’s diagnosis report. I will need the full packet complete with your child’s name and the doctor’s signature. I prefer this in PDF format
- A picture of the front and back of your child’s insurance card.
-A copy of our ABA intake paperwork completed and returned. This will be linked below for you to fill out. Once you fill it out and finish, it will automatically submit it to us.
-Link to the ABA paperwork:
-https://app.goformz.com/s/1MdG5YD51RRRvTsP6MQ
-Again, please do not hesitate to let me know if you have any questions!</t>
-  </si>
-  <si>
-    <t>[Brennan Behavior Group] Self Pay Consent</t>
-  </si>
-  <si>
-    <t>I'm processing your paperwork right now and see that you left the insurance section blank. If you'd like to proceed with self-pay please let me know! Below is the 2025 self-pay pricing list for our testing services. Billing for evaluations is reviewed with you and collected at the end of the process which is post testing.
-For self-pay patients a $300 Clinical Interview
-balance will be charged to the credit card on file on the day of the Clinical Interview appointment. The remaining evaluation balance will be charged to the card on file at the time of the feedback
-appointment. Educational testing will never be covered by insurance, which I’ve indicated in parentheses below.
-ADHD Testing — $2,460.00
-ASD Testing — $2,460.00-2,890.00
-Clergy/Seminarian Testing — $1950.00
-Psychoeducational/Full Evaluation — $3,305.00 ($1,750.00 is not covered by insurance)
-Gifted/IQ — $696.00 (not covered by insurance)
-Clinical Interview/Consultation (included in the above prices, but just the appointment alone) — $300.00 Billed after Clinical Interview.
-Please let me know if you have any questions and how you would like to proceed.
-Best,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Couples Therapy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Brennan Behavior Group] Couples Therapy </t>
-  </si>
-  <si>
-    <t>Hi there- 
-I see that you are interested in doing couples therapy. Our couples therapy is done by Ms. Lydia Jaunet, is an hour-long session, and is not covered by insurance. The cost of couples therapy is $250 a session. If you are interested in proceeding please have each partner complete the paperwork below and return it to this email address. Please don't hesitate to contact me if you have any questions or concerns!
-The link to fill out paperwork is below:
-https://app.goformz.com/s/Euj0YqkSiAugQqv6Ijr</t>
-  </si>
-  <si>
-    <t>Therapy Adult</t>
-  </si>
-  <si>
-    <t>[Brennan Behavior Group] Therapy Providers</t>
-  </si>
-  <si>
-    <t>Hi there-
-I am processing your paperwork and Ms. Amy Alvarez is our only adult therapist. She does accept insurance, but she has a waitlist of about 3-4 months. Amy has a special interest in prenatal and postpartum mental health, infant/toddler parenting support, infertility, and adoption. She also enjoys working with clients coping with divorce/custody, step-families, and career issues. Amy is LGBTQ allied and committed to social justice.
-Please let me know if you have any questions!
-Best,</t>
-  </si>
-  <si>
-    <t>Therapy Teens</t>
-  </si>
-  <si>
-    <t>Hi there-
-I am processing your paperwork and I wanted to reach out and give you some options as far as therapy providers. Unfortunately, we do not allow patients to be on multiple waitlists for providers at a time so once you review please let us know your preferred choice. 
-The first would be Ms. Lydia Jaunet. She does accept insurance, however, she is on a waitlist of about 4-6 months.  Lydia has experience in treating individuals, couples, and families who are struggling with disruptive behavior, conduct issues, ADD/ADHD, anxiety, depression, self-harming behaviors, and personality disorders.  Lydia strives to provide exceptional services through individual interventions based on her client’s needs, solution-focused treatment,  and cognitive-behavioral treatment models. 
-The other option would be Ms. Maya Gisclair. She does not accept insurance. Her self-pay rate is $138 for the very first session and any 60 minute sessions and $70 for each 30-minute session following that. She is on a waitlist of about 3-4 months. Maya addresses a wide range of psychological and behavioral issues through the use of functional communication training, solution-focused and client-centered treatment plans, as well as utilizing some Cognitive Behavioral Therapy (CBT) models. Her professional interests include ASD, disruptive behavior, conduct issues, ADD/ADHD, anxiety, depression, and self-injurious behaviors.
-The other option would be Ms. Amie Johnson. She is on a waitlist of 2-3 months, but she does not accept insurance. Her rates are $138 for the initial appointment, $138 for 60-minute sessions and $70 for 30-minute sessions. Amie’s interest is in providing therapeutic services to children, adolescents, and young-adults who are facing symptoms of depression, anxiety, ADD/ADHD, and ASD behaviors.                                                                                                                                                                              Please let me know if you have any other questions!
-Best,</t>
-  </si>
-  <si>
-    <t>Therapy Children</t>
-  </si>
-  <si>
-    <t>Hi there, 
-I am processing your paperwork and I wanted to reach out and give you some options as far as therapy providers. Unfortunately, we do not allow patients to be on multiple waitlists for providers at a time so once you review please let us know your preferred choice.  
-The first would be Ms. Lydia Jaunet. She does accept insurance, however, she is on a waitlist of about 4-6 months.  Lydia has experience in treating individuals, couples, and families who are struggling with disruptive behavior, conduct issues, ADD/ADHD, anxiety, depression, self-harming behaviors, and personality disorders.  Lydia strives to provide exceptional services through individual interventions based on her client’s needs, solution-focused treatment, and cognitive-behavioral treatment models. 
-The other option would be Ms. Maya Gisclair. She does not accept insurance. Her self-pay rate is $138 for the very first session and $70 for each 30-minute session following that.  She is on a waitlist of about 3-4 months. Maya addresses a wide range of psychological and behavioral issues through the use of functional communication training, solution-focused and client-centered treatment plans, as well as utilizing some Cognitive Behavioral Therapy (CBT) models. Her professional interests include ASD, disruptive behavior, conduct issues, ADD/ADHD, anxiety, depression, and self-injurious behaviors.                                                                                                                                                                                                                                            Please let me know if you have any other questions!
-Best,</t>
-  </si>
-  <si>
-    <t>Self Pay Blank</t>
-  </si>
-  <si>
-    <t>Self Pay Medicaid</t>
-  </si>
-  <si>
-    <t>I'm processing your paperwork right now and see that the insurance that you have provided us is an insurance we do not accept. If you'd like to proceed with self-pay please let me know! Below is the 2025 self-pay pricing list for our testing services. Billing for evaluations is reviewed with you and collected at the end of the process which is post testing.
-For self-pay patients a $300 Clinical Interview
-balance will be charged to the credit card on file on the day of the Clinical Interview appointment. The remaining evaluation balance will be charged to the card on file at the time of the feedback
-appointment. Educational testing will never be covered by insurance, which I’ve indicated in parentheses below.
-ADHD Testing — $2,460.00
-ASD Testing — $2,460.00-2,890.00
-Clergy/Seminarian Testing — $1950.00
-Psychoeducational/Full Evaluation — $3,305.00 ($1,750.00 is not covered by insurance)
-Gifted/IQ — $696.00 (not covered by insurance)
-Clinical Interview/Consultation (included in the above prices, but just the appointment alone) — $300.00 Billed after Clinical Interview.
-Please let me know if you have any questions and how you would like to proceed.
-Best,</t>
-  </si>
-  <si>
-    <t>[Brennan Behavior Group] Clerical Evaluation</t>
-  </si>
-  <si>
-    <t>Hi there,
-We see that you are interested in being evaluated by Dr. Gallagher. The paperwork attached to this email is our next step  in getting an appointment set up. It is preliminary information required for the evaluation. Once we receive the attached paperwork back, we will reach out with some appointment availability. Please let me know if you have any questions or concerns along the way!
-The link to the paperwork is below:
-https://app.goformz.com/s/9kY1p2UAnd4drPhNOHmw
-Best,</t>
-  </si>
-  <si>
-    <t>Hi there- &lt;br/&gt;
-I'm processing your paperwork and it looks like we're just missing your insurance information. If you could send me a photo/copy of the front and back of your card that would be great!
-&lt;br/&gt;
-Best,</t>
-  </si>
-  <si>
-    <t>Therapy</t>
+    <t>Hi there-&lt;br/&gt;&lt;br/&gt;I’m processing your paperwork and I see that you have insurance that we do not accept. If you’d like to proceed with self‑pay please let me know! Below is the 2025 self‑pay pricing list for our testing services. &lt;strong&gt;Billing for evaluations is reviewed with you and collected at the end of the process which is post testing.&lt;/strong&gt;&lt;br/&gt;&lt;br/&gt;For self‑pay patients, a $300 Clinical Interview balance will be charged to the credit card on file on the day of the Clinical Interview appointment. The remaining evaluation balance will be charged to the card on file at the time of the feedback appointment. Educational testing will never be covered by insurance, which I’ve indicated in parentheses below.&lt;br/&gt;&lt;br/&gt;&lt;mark&gt;ADHD Testing — $2,460.00&lt;/mark&gt;&lt;br/&gt;&lt;mark&gt;ASD Testing — $2,460.00–2,890.00&lt;/mark&gt;&lt;br/&gt;&lt;mark&gt;Clergy/Seminarian Testing — $1,950.00&lt;/mark&gt;&lt;br/&gt;&lt;mark&gt;Psychoeducational/Full Evaluation — $3,305.00 ( $1,750.00 is not covered by insurance)&lt;/mark&gt;&lt;br/&gt;&lt;mark&gt;Gifted/IQ — $696.00 (not covered by insurance)&lt;/mark&gt;&lt;br/&gt;&lt;mark&gt;Clinical Interview/Consultation (included in the above prices, but just the appointment alone) — $300.00 Billed after Clinical Interview&lt;/mark&gt;&lt;br/&gt;&lt;br/&gt;Please let me know if you have any questions and how you would like to proceed.&lt;br/&gt;&lt;br/&gt;Best,</t>
   </si>
 </sst>
 </file>
@@ -1520,7 +1490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1700,21 +1670,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2079,10 +2046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD75AEF6-164A-492E-8A25-0BD405F14B2D}">
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2185,13 +2152,13 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="52" t="s">
-        <v>323</v>
+        <v>275</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
         <v>263</v>
@@ -2202,18 +2169,9 @@
       <c r="G2" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="H2" s="52" t="s">
-        <v>277</v>
-      </c>
       <c r="I2" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="J2" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="K2" s="52" t="s">
-        <v>277</v>
-      </c>
       <c r="L2" s="52" t="s">
         <v>277</v>
       </c>
@@ -2223,13 +2181,22 @@
       <c r="N2" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="O2" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="P2" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="R2" s="52" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="52" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -2243,34 +2210,32 @@
       <c r="G3" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="H3" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="I3" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="L3" s="52" t="s">
+      <c r="J3" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="K3" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="L3" s="52"/>
       <c r="M3" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="N3" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="O3" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="P3" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="R3" s="52" t="s">
-        <v>277</v>
-      </c>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="Q3" s="52"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="52" t="s">
         <v>274</v>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -2296,17 +2261,23 @@
       <c r="K4" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52" t="s">
+      <c r="L4" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="N4" s="52"/>
-      <c r="O4" s="52"/>
-      <c r="Q4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="O4" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q4" s="52" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="52" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -2329,35 +2300,31 @@
       <c r="I5" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="J5" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="K5" s="52" t="s">
-        <v>277</v>
-      </c>
       <c r="L5" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="M5" s="52"/>
+      <c r="M5" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="N5" s="52" t="s">
         <v>277</v>
       </c>
       <c r="O5" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="Q5" s="52" t="s">
+      <c r="P5" s="52" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="52" t="s">
-        <v>273</v>
+        <v>321</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
       <c r="C6">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>263</v>
@@ -2377,28 +2344,25 @@
       <c r="L6" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="M6" s="52" t="s">
-        <v>277</v>
-      </c>
       <c r="N6" s="52" t="s">
         <v>277</v>
       </c>
       <c r="O6" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="P6" s="52" t="s">
+      <c r="S6" s="52" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="52" t="s">
-        <v>321</v>
+        <v>276</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
         <v>263</v>
@@ -2418,25 +2382,19 @@
       <c r="L7" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="N7" s="52" t="s">
-        <v>277</v>
-      </c>
       <c r="O7" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="S7" s="52" t="s">
-        <v>277</v>
-      </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="52" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
         <v>263</v>
@@ -2453,22 +2411,28 @@
       <c r="I8" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="J8" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="K8" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="L8" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="O8" s="52" t="s">
+      <c r="M8" s="52" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="52" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C9">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
         <v>263</v>
@@ -2491,10 +2455,11 @@
       <c r="K9" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="L9" s="52" t="s">
+      <c r="L9" s="52"/>
+      <c r="M9" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="M9" s="52" t="s">
+      <c r="O9" s="52" t="s">
         <v>277</v>
       </c>
     </row>
@@ -2503,10 +2468,10 @@
         <v>279</v>
       </c>
       <c r="B10">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
         <v>263</v>
@@ -2529,8 +2494,7 @@
       <c r="K10" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52" t="s">
+      <c r="L10" s="52" t="s">
         <v>277</v>
       </c>
       <c r="O10" s="52" t="s">
@@ -2539,13 +2503,13 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="52" t="s">
-        <v>279</v>
+        <v>27</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>263</v>
@@ -2571,19 +2535,28 @@
       <c r="L11" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="M11" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="N11" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="O11" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="P11" s="52" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="52" t="s">
-        <v>27</v>
+        <v>280</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
         <v>263</v>
@@ -2600,40 +2573,28 @@
       <c r="I12" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="J12" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="K12" s="52" t="s">
-        <v>277</v>
-      </c>
       <c r="L12" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="M12" s="52" t="s">
-        <v>277</v>
-      </c>
       <c r="N12" s="52" t="s">
         <v>277</v>
       </c>
       <c r="O12" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="P12" s="52" t="s">
-        <v>277</v>
-      </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="52" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>263</v>
+        <v>18</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>283</v>
       </c>
       <c r="F13" s="52" t="s">
         <v>277</v>
@@ -2641,31 +2602,29 @@
       <c r="G13" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="H13" s="52" t="s">
-        <v>277</v>
-      </c>
+      <c r="H13" s="52"/>
       <c r="I13" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="L13" s="52" t="s">
+      <c r="J13" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="N13" s="52" t="s">
+      <c r="T13" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="O13" s="52" t="s">
-        <v>277</v>
-      </c>
+      <c r="U13" s="52"/>
+      <c r="V13" s="52"/>
+      <c r="W13" s="52"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="52" t="s">
         <v>281</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C14">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>283</v>
@@ -2683,16 +2642,20 @@
       <c r="J14" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="T14" s="52" t="s">
+      <c r="T14" s="52"/>
+      <c r="U14" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="U14" s="52"/>
-      <c r="V14" s="52"/>
-      <c r="W14" s="52"/>
+      <c r="V14" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="W14" s="52" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B15">
         <v>18</v>
@@ -2709,30 +2672,28 @@
       <c r="G15" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="H15" s="52"/>
       <c r="I15" s="52" t="s">
         <v>277</v>
       </c>
       <c r="J15" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="T15" s="52"/>
-      <c r="U15" s="52" t="s">
+      <c r="K15" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="V15" s="52" t="s">
+      <c r="L15" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="W15" s="52" t="s">
+      <c r="T15" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="52" t="s">
-        <v>282</v>
+        <v>325</v>
       </c>
       <c r="B16">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>100</v>
@@ -2752,22 +2713,19 @@
       <c r="J16" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="K16" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="L16" s="52" t="s">
+      <c r="T16" s="52" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="52" t="s">
-        <v>325</v>
+        <v>287</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="D17" s="52" t="s">
         <v>283</v>
@@ -2775,28 +2733,22 @@
       <c r="F17" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="G17" s="52" t="s">
-        <v>277</v>
-      </c>
       <c r="I17" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="J17" s="52" t="s">
-        <v>277</v>
-      </c>
       <c r="T17" s="52" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="52" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C18">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D18" s="52" t="s">
         <v>283</v>
@@ -2813,24 +2765,42 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="52" t="s">
-        <v>288</v>
+        <v>323</v>
       </c>
       <c r="B19">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>23</v>
-      </c>
-      <c r="D19" s="52" t="s">
-        <v>283</v>
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>263</v>
       </c>
       <c r="F19" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="G19" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="H19" s="52" t="s">
+        <v>277</v>
+      </c>
       <c r="I19" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="T19" s="52" t="s">
+      <c r="J19" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="K19" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="L19" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="M19" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="N19" s="52" t="s">
         <v>277</v>
       </c>
     </row>
@@ -2839,12 +2809,6 @@
       <c r="D20" s="52"/>
       <c r="I20" s="52"/>
       <c r="T20" s="52"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="T21" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2859,7 +2823,7 @@
   <dimension ref="A1:AD1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="P6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="O29" sqref="O29"/>
@@ -35781,7 +35745,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="B15" t="s">
         <v>318</v>
@@ -35794,10 +35758,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21507685-9379-4BA4-B5A0-8A2C4C5B5836}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35807,7 +35771,7 @@
     <col min="3" max="3" width="75.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>339</v>
       </c>
@@ -35818,136 +35782,139 @@
         <v>341</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="71" t="s">
         <v>342</v>
       </c>
       <c r="B2" s="72" t="s">
         <v>343</v>
       </c>
-      <c r="C2" s="78" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="74" t="s">
+      <c r="C2" s="80" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="73" t="s">
+        <v>345</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>344</v>
+      </c>
+      <c r="C3" s="80" t="s">
+        <v>362</v>
+      </c>
+      <c r="D3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="78" t="s">
         <v>346</v>
-      </c>
-      <c r="B3" s="75" t="s">
-        <v>344</v>
-      </c>
-      <c r="C3" s="73" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="80" t="s">
-        <v>347</v>
       </c>
       <c r="B4" s="72" t="s">
         <v>344</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="80" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="79" t="s">
+        <v>347</v>
+      </c>
+      <c r="B5" s="72" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="81" t="s">
+      <c r="C5" s="80" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="232" x14ac:dyDescent="0.35">
+      <c r="A6" s="75" t="s">
+        <v>334</v>
+      </c>
+      <c r="B6" s="73" t="s">
         <v>349</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="C6" s="80" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="75" t="s">
+        <v>357</v>
+      </c>
+      <c r="B7" s="72" t="s">
         <v>350</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C7" s="80" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="77" t="s">
+        <v>358</v>
+      </c>
+      <c r="B8" s="72" t="s">
+        <v>350</v>
+      </c>
+      <c r="C8" s="80" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+      <c r="A9" s="73" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="76" t="s">
-        <v>334</v>
-      </c>
-      <c r="B6" s="74" t="s">
+      <c r="B9" s="73" t="s">
         <v>352</v>
       </c>
-      <c r="C6" s="73" t="s">
+      <c r="C9" s="80" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="73" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="76" t="s">
-        <v>366</v>
-      </c>
-      <c r="B7" s="72" t="s">
+      <c r="B10" s="73" t="s">
         <v>354</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C10" s="80" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="73" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="79" t="s">
-        <v>367</v>
-      </c>
-      <c r="B8" s="72" t="s">
+      <c r="B11" s="73" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="73" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="74" t="s">
+      <c r="C11" s="80" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="377" x14ac:dyDescent="0.35">
+      <c r="A12" s="73" t="s">
         <v>356</v>
       </c>
-      <c r="B9" s="74" t="s">
-        <v>357</v>
-      </c>
-      <c r="C9" s="73" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="74" t="s">
+      <c r="B12" s="73" t="s">
+        <v>354</v>
+      </c>
+      <c r="C12" s="76" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="203" x14ac:dyDescent="0.35">
+      <c r="A13" s="73" t="s">
+        <v>330</v>
+      </c>
+      <c r="B13" s="73" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="74" t="s">
-        <v>360</v>
-      </c>
-      <c r="C10" s="73" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="74" t="s">
-        <v>362</v>
-      </c>
-      <c r="B11" s="74" t="s">
-        <v>360</v>
-      </c>
-      <c r="C11" s="73" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="74" t="s">
-        <v>364</v>
-      </c>
-      <c r="B12" s="74" t="s">
-        <v>360</v>
-      </c>
-      <c r="C12" s="77" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="74" t="s">
-        <v>330</v>
-      </c>
-      <c r="B13" s="74" t="s">
-        <v>369</v>
-      </c>
-      <c r="C13" s="73" t="s">
-        <v>370</v>
+      <c r="C13" s="80" t="s">
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>